<commit_message>
revised group membership beause of miscommunication
</commit_message>
<xml_diff>
--- a/G3.xlsx
+++ b/G3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cjd032/Documents/Teaching/2018-2019/CMPT370/Documents/Teams/Team Exports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD0119DA-D5A5-E947-8B56-C9B8C736E623}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F89B103-A912-6547-9A7F-6F9FEDB2F10E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11980" yWindow="7560" windowWidth="13620" windowHeight="8440" xr2:uid="{5D3BA78C-8A9F-6942-B3AB-40A20E49EC63}"/>
+    <workbookView xWindow="6380" yWindow="2620" windowWidth="18060" windowHeight="13380" xr2:uid="{5D3BA78C-8A9F-6942-B3AB-40A20E49EC63}"/>
   </bookViews>
   <sheets>
     <sheet name="Team G3" sheetId="1" r:id="rId1"/>
@@ -24,8 +24,32 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Microsoft Office User</author>
+  </authors>
+  <commentList>
+    <comment ref="G8" authorId="0" shapeId="0" xr:uid="{3636B24C-BCCC-1044-82D5-48CC6AA1E85D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="10"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>oll096, after the fact, punted on lmi955</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="253" uniqueCount="106">
   <si>
     <t>GIT?</t>
   </si>
@@ -322,13 +346,34 @@
   </si>
   <si>
     <t xml:space="preserve">I work part time usually 20+ hours a week. My math and theory skills are pretty weak, I've done poorly in related courses. </t>
+  </si>
+  <si>
+    <t>Lacoste-Bouchet</t>
+  </si>
+  <si>
+    <t>Olivier</t>
+  </si>
+  <si>
+    <t>oll096</t>
+  </si>
+  <si>
+    <t>lmi955</t>
+  </si>
+  <si>
+    <t>ENG</t>
+  </si>
+  <si>
+    <t>Competent</t>
+  </si>
+  <si>
+    <t>Currently taking 5 classes</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -378,8 +423,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="CMU Typewriter Text Regular"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="9">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -425,6 +483,18 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -534,163 +604,856 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="68">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B0F0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color auto="1"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -999,894 +1762,1001 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3332F48A-568F-FA4F-A8E4-03474E574E4B}">
-  <dimension ref="A1:AT7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3332F48A-568F-FA4F-A8E4-03474E574E4B}">
+  <dimension ref="A1:AX8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD12"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="10.83203125" style="24"/>
-    <col min="3" max="3" width="16.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="11"/>
-    <col min="5" max="5" width="5.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="7.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="5.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="23" width="10.83203125" style="11"/>
-    <col min="24" max="26" width="10.83203125" style="24"/>
-    <col min="27" max="27" width="10.1640625" style="48" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="10.83203125" style="11"/>
-    <col min="29" max="29" width="10.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.1640625" style="48" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="10.83203125" style="11"/>
-    <col min="32" max="32" width="14.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="10.83203125" style="48"/>
-    <col min="34" max="34" width="13.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="35" max="39" width="14.1640625" style="11" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="9.5" style="11" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="10.83203125" style="11"/>
-    <col min="42" max="42" width="13.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="43" max="44" width="10.83203125" style="11"/>
-    <col min="45" max="45" width="8.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="54.83203125" style="49" customWidth="1"/>
-    <col min="47" max="16384" width="10.83203125" style="11"/>
+    <col min="1" max="2" width="10.83203125" style="12"/>
+    <col min="3" max="3" width="16.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="5"/>
+    <col min="5" max="5" width="5.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="23" width="10.83203125" style="5"/>
+    <col min="24" max="26" width="10.83203125" style="12"/>
+    <col min="27" max="27" width="10.1640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="10.83203125" style="5"/>
+    <col min="29" max="29" width="10.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.1640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="10.83203125" style="5"/>
+    <col min="32" max="32" width="14.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.83203125" style="36"/>
+    <col min="34" max="34" width="13.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="35" max="39" width="14.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="9.5" style="5" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="10.83203125" style="5"/>
+    <col min="42" max="42" width="13.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="43" max="44" width="10.83203125" style="5"/>
+    <col min="45" max="45" width="8.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="54.83203125" style="37" customWidth="1"/>
+    <col min="47" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:46">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:50">
+      <c r="A1" s="48" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="G1" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="41"/>
+      <c r="I1" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3" t="s">
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="4" t="s">
+      <c r="L1" s="42" t="s">
         <v>8</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="M1" s="39" t="s">
         <v>9</v>
       </c>
-      <c r="N1" s="5" t="s">
+      <c r="N1" s="39" t="s">
         <v>10</v>
       </c>
-      <c r="O1" s="6"/>
-      <c r="P1" s="6"/>
-      <c r="Q1" s="6"/>
-      <c r="R1" s="6"/>
-      <c r="S1" s="6"/>
-      <c r="T1" s="6"/>
-      <c r="U1" s="6"/>
-      <c r="V1" s="6"/>
-      <c r="W1" s="4"/>
-      <c r="X1" s="7" t="s">
+      <c r="O1" s="40"/>
+      <c r="P1" s="40"/>
+      <c r="Q1" s="40"/>
+      <c r="R1" s="40"/>
+      <c r="S1" s="40"/>
+      <c r="T1" s="40"/>
+      <c r="U1" s="40"/>
+      <c r="V1" s="40"/>
+      <c r="W1" s="42"/>
+      <c r="X1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="Y1" s="8" t="s">
+      <c r="Y1" s="46" t="s">
         <v>12</v>
       </c>
-      <c r="Z1" s="7" t="s">
+      <c r="Z1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AA1" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="AB1" s="2"/>
-      <c r="AC1" s="4"/>
-      <c r="AD1" s="5" t="s">
+      <c r="AB1" s="41"/>
+      <c r="AC1" s="42"/>
+      <c r="AD1" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="AE1" s="6"/>
-      <c r="AF1" s="6"/>
-      <c r="AG1" s="5" t="s">
+      <c r="AE1" s="40"/>
+      <c r="AF1" s="40"/>
+      <c r="AG1" s="39" t="s">
         <v>16</v>
       </c>
-      <c r="AH1" s="6"/>
-      <c r="AI1" s="6"/>
-      <c r="AJ1" s="6"/>
-      <c r="AK1" s="2" t="s">
+      <c r="AH1" s="40"/>
+      <c r="AI1" s="40"/>
+      <c r="AJ1" s="40"/>
+      <c r="AK1" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="AL1" s="2"/>
-      <c r="AM1" s="2"/>
-      <c r="AN1" s="2" t="s">
+      <c r="AL1" s="41"/>
+      <c r="AM1" s="41"/>
+      <c r="AN1" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="AO1" s="2"/>
-      <c r="AP1" s="2"/>
-      <c r="AQ1" s="2" t="s">
+      <c r="AO1" s="41"/>
+      <c r="AP1" s="41"/>
+      <c r="AQ1" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="AR1" s="4"/>
-      <c r="AS1" s="9" t="s">
+      <c r="AR1" s="42"/>
+      <c r="AS1" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AT1" s="10"/>
+      <c r="AT1" s="4"/>
     </row>
-    <row r="2" spans="1:46" s="23" customFormat="1" ht="18" thickBot="1">
-      <c r="A2" s="12"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="14" t="s">
+    <row r="2" spans="1:50" s="11" customFormat="1" ht="18" thickBot="1">
+      <c r="A2" s="49"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="E2" s="14" t="s">
+      <c r="E2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="14" t="s">
+      <c r="F2" s="43"/>
+      <c r="G2" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H2" s="14" t="s">
+      <c r="H2" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I2" s="15"/>
-      <c r="J2" s="15"/>
-      <c r="K2" s="14" t="s">
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
+      <c r="K2" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="L2" s="16"/>
-      <c r="M2" s="17"/>
-      <c r="N2" s="18">
+      <c r="L2" s="44"/>
+      <c r="M2" s="45"/>
+      <c r="N2" s="7">
         <v>215</v>
       </c>
-      <c r="O2" s="14">
+      <c r="O2" s="6">
         <v>260</v>
       </c>
-      <c r="P2" s="14">
+      <c r="P2" s="6">
         <v>280</v>
       </c>
-      <c r="Q2" s="14">
+      <c r="Q2" s="6">
         <v>306</v>
       </c>
-      <c r="R2" s="14">
+      <c r="R2" s="6">
         <v>317</v>
       </c>
-      <c r="S2" s="14">
+      <c r="S2" s="6">
         <v>332</v>
       </c>
-      <c r="T2" s="14">
+      <c r="T2" s="6">
         <v>340</v>
       </c>
-      <c r="U2" s="14">
+      <c r="U2" s="6">
         <v>350</v>
       </c>
-      <c r="V2" s="14">
+      <c r="V2" s="6">
         <v>360</v>
       </c>
-      <c r="W2" s="14">
+      <c r="W2" s="6">
         <v>381</v>
       </c>
-      <c r="X2" s="19" t="s">
+      <c r="X2" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="Y2" s="20"/>
-      <c r="Z2" s="19" t="s">
+      <c r="Y2" s="47"/>
+      <c r="Z2" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="AA2" s="18" t="s">
+      <c r="AA2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="AB2" s="14" t="s">
+      <c r="AB2" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="AC2" s="14" t="s">
+      <c r="AC2" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="AD2" s="18" t="s">
+      <c r="AD2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="AE2" s="14" t="s">
+      <c r="AE2" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="AF2" s="14" t="s">
+      <c r="AF2" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="AG2" s="18" t="s">
+      <c r="AG2" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="AH2" s="14" t="s">
+      <c r="AH2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="AI2" s="14" t="s">
+      <c r="AI2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="AJ2" s="14" t="s">
+      <c r="AJ2" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="AK2" s="14" t="s">
+      <c r="AK2" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="AL2" s="14" t="s">
+      <c r="AL2" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="AM2" s="14" t="s">
+      <c r="AM2" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="AN2" s="18" t="s">
+      <c r="AN2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="AO2" s="14" t="s">
+      <c r="AO2" s="6" t="s">
         <v>43</v>
       </c>
-      <c r="AP2" s="14" t="s">
+      <c r="AP2" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="AQ2" s="18" t="s">
+      <c r="AQ2" s="7" t="s">
         <v>45</v>
       </c>
-      <c r="AR2" s="18" t="s">
+      <c r="AR2" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="AS2" s="21" t="s">
+      <c r="AS2" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="AT2" s="22" t="s">
+      <c r="AT2" s="10" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:46" ht="51">
-      <c r="A3" s="24" t="s">
+    <row r="3" spans="1:50" ht="51">
+      <c r="A3" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="14" t="s">
         <v>81</v>
       </c>
-      <c r="D3" s="26" t="s">
+      <c r="D3" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="15" t="s">
         <v>82</v>
       </c>
-      <c r="G3" s="26" t="s">
+      <c r="G3" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="H3" s="26" t="s">
+      <c r="H3" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="I3" s="26" t="s">
+      <c r="I3" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="K3" s="26" t="s">
+      <c r="K3" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="L3" s="28" t="s">
+      <c r="L3" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="M3" s="39" t="s">
+      <c r="M3" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="N3" s="29" t="s">
+      <c r="N3" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="O3" s="32" t="s">
+      <c r="O3" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="P3" s="32" t="s">
+      <c r="P3" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="Q3" s="31" t="s">
+      <c r="Q3" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="R3" s="32" t="s">
+      <c r="R3" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="S3" s="26"/>
-      <c r="T3" s="26"/>
-      <c r="U3" s="26"/>
-      <c r="V3" s="26"/>
-      <c r="W3" s="26"/>
-      <c r="X3" s="45" t="s">
+      <c r="S3" s="14"/>
+      <c r="T3" s="14"/>
+      <c r="U3" s="14"/>
+      <c r="V3" s="14"/>
+      <c r="W3" s="14"/>
+      <c r="X3" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="Y3" s="33"/>
-      <c r="Z3" s="33"/>
-      <c r="AA3" s="42" t="s">
+      <c r="Y3" s="21"/>
+      <c r="Z3" s="21"/>
+      <c r="AA3" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="AB3" s="43" t="s">
+      <c r="AB3" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="AC3" s="43" t="s">
+      <c r="AC3" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="AD3" s="46" t="s">
+      <c r="AD3" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="AE3" s="32" t="s">
+      <c r="AE3" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="AF3" s="35" t="s">
+      <c r="AF3" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="AG3" s="46" t="s">
+      <c r="AG3" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="AH3" s="35" t="s">
+      <c r="AH3" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="AI3" s="35" t="s">
+      <c r="AI3" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="AJ3" s="35" t="s">
+      <c r="AJ3" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="AK3" s="35" t="s">
+      <c r="AK3" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="AL3" s="32" t="s">
+      <c r="AL3" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="AM3" s="35" t="s">
+      <c r="AM3" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="AN3" s="38">
+      <c r="AN3" s="26">
         <v>1000</v>
       </c>
-      <c r="AO3" s="26">
+      <c r="AO3" s="14">
         <v>1500</v>
       </c>
-      <c r="AP3" s="26">
+      <c r="AP3" s="14">
         <v>3</v>
       </c>
-      <c r="AQ3" s="29" t="s">
+      <c r="AQ3" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="AR3" s="29" t="s">
+      <c r="AR3" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="AS3" s="47">
+      <c r="AS3" s="35">
         <v>1</v>
       </c>
-      <c r="AT3" s="41" t="s">
+      <c r="AT3" s="29" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="4" spans="1:46" ht="18">
-      <c r="A4" s="24" t="s">
+    <row r="4" spans="1:50" ht="18">
+      <c r="A4" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="14" t="s">
         <v>84</v>
       </c>
-      <c r="D4" s="26" t="s">
+      <c r="D4" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="E4" s="26" t="s">
+      <c r="E4" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="F4" s="27" t="s">
+      <c r="F4" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="G4" s="26" t="s">
+      <c r="G4" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="H4" s="26" t="s">
+      <c r="H4" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="I4" s="26" t="s">
+      <c r="I4" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="J4" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="K4" s="26" t="s">
+      <c r="K4" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="L4" s="28" t="s">
+      <c r="L4" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="M4" s="30" t="s">
+      <c r="M4" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="N4" s="29" t="s">
+      <c r="N4" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="O4" s="31" t="s">
+      <c r="O4" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="P4" s="31" t="s">
+      <c r="P4" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="Q4" s="31" t="s">
+      <c r="Q4" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="R4" s="31" t="s">
+      <c r="R4" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="S4" s="26"/>
-      <c r="T4" s="26"/>
-      <c r="U4" s="26"/>
-      <c r="V4" s="26"/>
-      <c r="W4" s="26"/>
-      <c r="X4" s="45" t="s">
+      <c r="S4" s="14"/>
+      <c r="T4" s="14"/>
+      <c r="U4" s="14"/>
+      <c r="V4" s="14"/>
+      <c r="W4" s="14"/>
+      <c r="X4" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="Y4" s="33"/>
-      <c r="Z4" s="33"/>
-      <c r="AA4" s="42" t="s">
+      <c r="Y4" s="21"/>
+      <c r="Z4" s="21"/>
+      <c r="AA4" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="AB4" s="43" t="s">
+      <c r="AB4" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="AC4" s="43" t="s">
+      <c r="AC4" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="AD4" s="29" t="s">
+      <c r="AD4" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="AE4" s="37" t="s">
+      <c r="AE4" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="AF4" s="32" t="s">
+      <c r="AF4" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="AG4" s="36" t="s">
+      <c r="AG4" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="AH4" s="37" t="s">
+      <c r="AH4" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="AI4" s="35" t="s">
+      <c r="AI4" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="AJ4" s="35" t="s">
+      <c r="AJ4" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="AK4" s="37" t="s">
+      <c r="AK4" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="AL4" s="32" t="s">
+      <c r="AL4" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="AM4" s="32" t="s">
+      <c r="AM4" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="AN4" s="38">
+      <c r="AN4" s="26">
         <v>400</v>
       </c>
-      <c r="AO4" s="26">
+      <c r="AO4" s="14">
         <v>1500</v>
       </c>
-      <c r="AP4" s="26">
+      <c r="AP4" s="14">
         <v>10</v>
       </c>
-      <c r="AQ4" s="29" t="s">
+      <c r="AQ4" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="AR4" s="29" t="s">
+      <c r="AR4" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="AS4" s="40">
+      <c r="AS4" s="28">
         <v>2</v>
       </c>
-      <c r="AT4" s="41"/>
+      <c r="AT4" s="29"/>
     </row>
-    <row r="5" spans="1:46" ht="18">
-      <c r="A5" s="24" t="s">
+    <row r="5" spans="1:50" ht="18">
+      <c r="A5" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="B5" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="26" t="s">
+      <c r="D5" s="14" t="s">
         <v>89</v>
       </c>
-      <c r="E5" s="26" t="s">
+      <c r="E5" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="F5" s="27" t="s">
+      <c r="F5" s="15" t="s">
         <v>90</v>
       </c>
-      <c r="G5" s="26" t="s">
+      <c r="G5" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="H5" s="26" t="s">
+      <c r="H5" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="I5" s="26" t="s">
+      <c r="I5" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="J5" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="K5" s="26" t="s">
+      <c r="K5" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="L5" s="28" t="s">
+      <c r="L5" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="M5" s="30" t="s">
+      <c r="M5" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="N5" s="29" t="s">
+      <c r="N5" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="O5" s="32" t="s">
+      <c r="O5" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="P5" s="32" t="s">
+      <c r="P5" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="Q5" s="26"/>
-      <c r="R5" s="26"/>
-      <c r="S5" s="26"/>
-      <c r="T5" s="26"/>
-      <c r="U5" s="26"/>
-      <c r="V5" s="26"/>
-      <c r="W5" s="26"/>
-      <c r="X5" s="45" t="s">
+      <c r="Q5" s="14"/>
+      <c r="R5" s="14"/>
+      <c r="S5" s="14"/>
+      <c r="T5" s="14"/>
+      <c r="U5" s="14"/>
+      <c r="V5" s="14"/>
+      <c r="W5" s="14"/>
+      <c r="X5" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="Y5" s="33"/>
-      <c r="Z5" s="33"/>
-      <c r="AA5" s="42" t="s">
+      <c r="Y5" s="21"/>
+      <c r="Z5" s="21"/>
+      <c r="AA5" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="AB5" s="43" t="s">
+      <c r="AB5" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="AC5" s="32" t="s">
+      <c r="AC5" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="AD5" s="29" t="s">
+      <c r="AD5" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="AE5" s="32" t="s">
+      <c r="AE5" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="AF5" s="31" t="s">
+      <c r="AF5" s="19" t="s">
         <v>64</v>
       </c>
-      <c r="AG5" s="46" t="s">
+      <c r="AG5" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="AH5" s="35" t="s">
+      <c r="AH5" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="AI5" s="32" t="s">
+      <c r="AI5" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="AJ5" s="35" t="s">
+      <c r="AJ5" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="AK5" s="35" t="s">
+      <c r="AK5" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="AL5" s="32" t="s">
+      <c r="AL5" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="AM5" s="32" t="s">
+      <c r="AM5" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="AN5" s="38">
+      <c r="AN5" s="26">
         <v>500</v>
       </c>
-      <c r="AO5" s="26">
+      <c r="AO5" s="14">
         <v>0</v>
       </c>
-      <c r="AP5" s="26">
+      <c r="AP5" s="14">
         <v>1</v>
       </c>
-      <c r="AQ5" s="30" t="s">
+      <c r="AQ5" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="AR5" s="29" t="s">
+      <c r="AR5" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="AS5" s="50" t="s">
+      <c r="AS5" s="38" t="s">
         <v>78</v>
       </c>
-      <c r="AT5" s="41"/>
+      <c r="AT5" s="29"/>
     </row>
-    <row r="6" spans="1:46" ht="119">
-      <c r="A6" s="44"/>
-      <c r="B6" s="25" t="s">
+    <row r="6" spans="1:50" ht="119">
+      <c r="A6" s="32"/>
+      <c r="B6" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="14" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="26" t="s">
+      <c r="D6" s="14" t="s">
         <v>92</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="G6" s="26" t="s">
+      <c r="G6" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="I6" s="26" t="s">
+      <c r="I6" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="J6" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="K6" s="26" t="s">
+      <c r="K6" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="L6" s="28" t="s">
+      <c r="L6" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="M6" s="39" t="s">
+      <c r="M6" s="27" t="s">
         <v>69</v>
       </c>
-      <c r="N6" s="30" t="s">
+      <c r="N6" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="O6" s="31" t="s">
+      <c r="O6" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="P6" s="32" t="s">
+      <c r="P6" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="Q6" s="26"/>
-      <c r="R6" s="32" t="s">
+      <c r="Q6" s="14"/>
+      <c r="R6" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="S6" s="26"/>
-      <c r="T6" s="32" t="s">
+      <c r="S6" s="14"/>
+      <c r="T6" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="U6" s="31" t="s">
+      <c r="U6" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="V6" s="26"/>
-      <c r="W6" s="31" t="s">
+      <c r="V6" s="14"/>
+      <c r="W6" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="X6" s="45" t="s">
+      <c r="X6" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="Y6" s="33"/>
-      <c r="Z6" s="33"/>
-      <c r="AA6" s="42" t="s">
+      <c r="Y6" s="21"/>
+      <c r="Z6" s="21"/>
+      <c r="AA6" s="30" t="s">
         <v>60</v>
       </c>
-      <c r="AB6" s="43" t="s">
+      <c r="AB6" s="31" t="s">
         <v>60</v>
       </c>
-      <c r="AC6" s="32" t="s">
+      <c r="AC6" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AD6" s="29" t="s">
+      <c r="AD6" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="AE6" s="32" t="s">
+      <c r="AE6" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="AF6" s="35" t="s">
+      <c r="AF6" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="AG6" s="46" t="s">
+      <c r="AG6" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="AH6" s="37" t="s">
+      <c r="AH6" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="AI6" s="34" t="s">
+      <c r="AI6" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="AJ6" s="35" t="s">
+      <c r="AJ6" s="23" t="s">
         <v>56</v>
       </c>
-      <c r="AK6" s="32" t="s">
+      <c r="AK6" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="AL6" s="32" t="s">
+      <c r="AL6" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="AM6" s="32" t="s">
+      <c r="AM6" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="AN6" s="38">
+      <c r="AN6" s="26">
         <v>500</v>
       </c>
-      <c r="AO6" s="26">
+      <c r="AO6" s="14">
         <v>1000</v>
       </c>
-      <c r="AP6" s="26"/>
-      <c r="AQ6" s="29" t="s">
+      <c r="AP6" s="14"/>
+      <c r="AQ6" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="AR6" s="29" t="s">
+      <c r="AR6" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="AS6" s="47">
+      <c r="AS6" s="35">
         <v>1</v>
       </c>
-      <c r="AT6" s="41" t="s">
+      <c r="AT6" s="29" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="7" spans="1:46" ht="34">
-      <c r="A7" s="24" t="s">
+    <row r="7" spans="1:50" ht="34">
+      <c r="A7" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="14" t="s">
         <v>95</v>
       </c>
-      <c r="D7" s="26" t="s">
+      <c r="D7" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="E7" s="26" t="s">
+      <c r="E7" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F7" s="27" t="s">
+      <c r="F7" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="G7" s="26" t="s">
+      <c r="G7" s="14" t="s">
         <v>58</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="I7" s="26" t="s">
+      <c r="I7" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="14" t="s">
         <v>67</v>
       </c>
-      <c r="K7" s="26" t="s">
+      <c r="K7" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="L7" s="28" t="s">
+      <c r="L7" s="16" t="s">
         <v>61</v>
       </c>
-      <c r="M7" s="29" t="s">
+      <c r="M7" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="N7" s="29" t="s">
+      <c r="N7" s="17" t="s">
         <v>54</v>
       </c>
-      <c r="O7" s="32" t="s">
+      <c r="O7" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="P7" s="31" t="s">
+      <c r="P7" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="Q7" s="26"/>
-      <c r="R7" s="31" t="s">
+      <c r="Q7" s="14"/>
+      <c r="R7" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="S7" s="26"/>
-      <c r="T7" s="26"/>
-      <c r="U7" s="26"/>
-      <c r="V7" s="32" t="s">
+      <c r="S7" s="14"/>
+      <c r="T7" s="14"/>
+      <c r="U7" s="14"/>
+      <c r="V7" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="W7" s="32" t="s">
+      <c r="W7" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="X7" s="45" t="s">
+      <c r="X7" s="33" t="s">
         <v>68</v>
       </c>
-      <c r="Y7" s="33"/>
-      <c r="Z7" s="33"/>
-      <c r="AA7" s="29" t="s">
+      <c r="Y7" s="21"/>
+      <c r="Z7" s="21"/>
+      <c r="AA7" s="17" t="s">
         <v>70</v>
       </c>
-      <c r="AB7" s="32" t="s">
+      <c r="AB7" s="20" t="s">
         <v>70</v>
       </c>
-      <c r="AC7" s="37" t="s">
+      <c r="AC7" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="AD7" s="29" t="s">
+      <c r="AD7" s="17" t="s">
         <v>55</v>
       </c>
-      <c r="AE7" s="32" t="s">
+      <c r="AE7" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="AF7" s="32" t="s">
+      <c r="AF7" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="AG7" s="36" t="s">
+      <c r="AG7" s="24" t="s">
         <v>57</v>
       </c>
-      <c r="AH7" s="37" t="s">
+      <c r="AH7" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="AI7" s="32" t="s">
+      <c r="AI7" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="AJ7" s="37" t="s">
+      <c r="AJ7" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="AK7" s="37" t="s">
+      <c r="AK7" s="25" t="s">
         <v>57</v>
       </c>
-      <c r="AL7" s="34" t="s">
+      <c r="AL7" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="AM7" s="32" t="s">
+      <c r="AM7" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="AN7" s="38">
+      <c r="AN7" s="26">
         <v>400</v>
       </c>
-      <c r="AO7" s="26">
+      <c r="AO7" s="14">
         <v>0</v>
       </c>
-      <c r="AP7" s="26">
+      <c r="AP7" s="14">
         <v>0</v>
       </c>
-      <c r="AQ7" s="29" t="s">
+      <c r="AQ7" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="AR7" s="29" t="s">
+      <c r="AR7" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="AS7" s="40">
+      <c r="AS7" s="28">
         <v>2</v>
       </c>
-      <c r="AT7" s="41" t="s">
+      <c r="AT7" s="29" t="s">
         <v>98</v>
+      </c>
+    </row>
+    <row r="8" spans="1:50" ht="18">
+      <c r="B8" s="58" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8" t="s">
+        <v>100</v>
+      </c>
+      <c r="E8"/>
+      <c r="F8" s="51" t="s">
+        <v>101</v>
+      </c>
+      <c r="G8" s="52" t="s">
+        <v>102</v>
+      </c>
+      <c r="H8" s="51"/>
+      <c r="I8" t="s">
+        <v>58</v>
+      </c>
+      <c r="J8" s="53" t="s">
+        <v>77</v>
+      </c>
+      <c r="K8" t="s">
+        <v>66</v>
+      </c>
+      <c r="L8" t="s">
+        <v>49</v>
+      </c>
+      <c r="M8" t="s">
+        <v>103</v>
+      </c>
+      <c r="N8" s="54" t="s">
+        <v>51</v>
+      </c>
+      <c r="O8" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="P8" s="55"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8"/>
+      <c r="W8"/>
+      <c r="X8"/>
+      <c r="Y8"/>
+      <c r="Z8" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="AA8" s="55"/>
+      <c r="AB8" s="55"/>
+      <c r="AC8" t="s">
+        <v>70</v>
+      </c>
+      <c r="AD8" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE8" t="s">
+        <v>104</v>
+      </c>
+      <c r="AF8" s="55" t="s">
+        <v>55</v>
+      </c>
+      <c r="AG8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AH8" t="s">
+        <v>62</v>
+      </c>
+      <c r="AI8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AJ8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>56</v>
+      </c>
+      <c r="AL8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AN8" t="s">
+        <v>55</v>
+      </c>
+      <c r="AO8" t="s">
+        <v>57</v>
+      </c>
+      <c r="AP8" s="55">
+        <v>500</v>
+      </c>
+      <c r="AQ8"/>
+      <c r="AR8">
+        <v>2</v>
+      </c>
+      <c r="AS8" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="AT8" s="56" t="s">
+        <v>68</v>
+      </c>
+      <c r="AU8" s="57">
+        <v>2</v>
+      </c>
+      <c r="AV8" t="s">
+        <v>102</v>
+      </c>
+      <c r="AW8"/>
+      <c r="AX8" t="s">
+        <v>105</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="AD1:AF1"/>
-    <mergeCell ref="AG1:AJ1"/>
-    <mergeCell ref="AK1:AM1"/>
-    <mergeCell ref="AN1:AP1"/>
-    <mergeCell ref="AQ1:AR1"/>
-    <mergeCell ref="J1:J2"/>
-    <mergeCell ref="L1:L2"/>
-    <mergeCell ref="M1:M2"/>
-    <mergeCell ref="N1:W1"/>
-    <mergeCell ref="Y1:Y2"/>
     <mergeCell ref="AA1:AC1"/>
     <mergeCell ref="A1:A2"/>
     <mergeCell ref="B1:B2"/>
@@ -1894,7 +2764,134 @@
     <mergeCell ref="F1:F2"/>
     <mergeCell ref="G1:H1"/>
     <mergeCell ref="I1:I2"/>
+    <mergeCell ref="J1:J2"/>
+    <mergeCell ref="L1:L2"/>
+    <mergeCell ref="M1:M2"/>
+    <mergeCell ref="N1:W1"/>
+    <mergeCell ref="Y1:Y2"/>
+    <mergeCell ref="AD1:AF1"/>
+    <mergeCell ref="AG1:AJ1"/>
+    <mergeCell ref="AK1:AM1"/>
+    <mergeCell ref="AN1:AP1"/>
+    <mergeCell ref="AQ1:AR1"/>
   </mergeCells>
+  <conditionalFormatting sqref="AC8:AE8">
+    <cfRule type="containsText" dxfId="33" priority="29" operator="containsText" text="Limited">
+      <formula>NOT(ISERROR(SEARCH("Limited",AC8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="32" priority="30" operator="containsText" text="Modest">
+      <formula>NOT(ISERROR(SEARCH("Modest",AC8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="31" priority="31" operator="containsText" text="Competent">
+      <formula>NOT(ISERROR(SEARCH("Competent",AC8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="30" priority="32" operator="containsText" text="Good">
+      <formula>NOT(ISERROR(SEARCH("Good",AC8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="29" priority="33" operator="containsText" text="Very Good">
+      <formula>NOT(ISERROR(SEARCH("Very Good",AC8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="28" priority="34" operator="containsText" text="Fluent">
+      <formula>NOT(ISERROR(SEARCH("Fluent",AC8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="P8:Y8">
+    <cfRule type="containsText" dxfId="27" priority="27" operator="containsText" text="STRONG">
+      <formula>NOT(ISERROR(SEARCH("STRONG",P8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="26" priority="28" operator="containsText" text="WEAK">
+      <formula>NOT(ISERROR(SEARCH("WEAK",P8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AS8 O8">
+    <cfRule type="containsText" dxfId="25" priority="22" operator="containsText" text="Exceptional">
+      <formula>NOT(ISERROR(SEARCH("Exceptional",O8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="24" priority="23" operator="containsText" text="Excellent">
+      <formula>NOT(ISERROR(SEARCH("Excellent",O8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="23" priority="24" operator="containsText" text="Good">
+      <formula>NOT(ISERROR(SEARCH("Good",O8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="22" priority="25" operator="containsText" text="Satisfactory">
+      <formula>NOT(ISERROR(SEARCH("Satisfactory",O8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="21" priority="26" operator="containsText" text="Minimal">
+      <formula>NOT(ISERROR(SEARCH("Minimal",O8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AT8">
+    <cfRule type="containsText" dxfId="20" priority="17" operator="containsText" text="&lt;5">
+      <formula>NOT(ISERROR(SEARCH("&lt;5",AT8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="19" priority="18" operator="containsText" text="5--10">
+      <formula>NOT(ISERROR(SEARCH("5--10",AT8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="18" priority="19" operator="containsText" text="10--15">
+      <formula>NOT(ISERROR(SEARCH("10--15",AT8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="17" priority="20" operator="containsText" text="15--25">
+      <formula>NOT(ISERROR(SEARCH("15--25",AT8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="16" priority="21" operator="containsText" text="&gt;25">
+      <formula>NOT(ISERROR(SEARCH("&gt;25",AT8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AU8">
+    <cfRule type="containsText" dxfId="15" priority="12" operator="containsText" text="&gt;3">
+      <formula>NOT(ISERROR(SEARCH("&gt;3",AU8)))</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="14" priority="13" operator="equal">
+      <formula>3</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="13" priority="14" operator="equal">
+      <formula>2</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="12" priority="15" operator="equal">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="11" priority="16" operator="equal">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="AF8:AO8">
+    <cfRule type="containsText" dxfId="10" priority="6" operator="containsText" text="Industry">
+      <formula>NOT(ISERROR(SEARCH("Industry",AF8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="7" operator="containsText" text="Regularly">
+      <formula>NOT(ISERROR(SEARCH("Regularly",AF8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="8" priority="8" operator="containsText" text="Used in Courses">
+      <formula>NOT(ISERROR(SEARCH("Used in Courses",AF8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="9" operator="containsText" text="Saw in Courses">
+      <formula>NOT(ISERROR(SEARCH("Saw in Courses",AF8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="6" priority="10" operator="containsText" text="Heard of">
+      <formula>NOT(ISERROR(SEARCH("Heard of",AF8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="5" priority="11" operator="containsText" text="Huh?">
+      <formula>NOT(ISERROR(SEARCH("Huh?",AF8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="Z8">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="&lt;5">
+      <formula>NOT(ISERROR(SEARCH("&lt;5",Z8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="5--10">
+      <formula>NOT(ISERROR(SEARCH("5--10",Z8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="2" priority="3" operator="containsText" text="10--15">
+      <formula>NOT(ISERROR(SEARCH("10--15",Z8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="4" operator="containsText" text="15--20">
+      <formula>NOT(ISERROR(SEARCH("15--20",Z8)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="0" priority="5" operator="containsText" text="&gt;20">
+      <formula>NOT(ISERROR(SEARCH("&gt;20",Z8)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>